<commit_message>
Files related to DB Modifications
</commit_message>
<xml_diff>
--- a/MigrationRenamer.xlsx
+++ b/MigrationRenamer.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>Files</t>
   </si>
@@ -44,61 +44,67 @@
     <t>CMD</t>
   </si>
   <si>
-    <t>2020_10_05_000001_update_users_table.php</t>
-  </si>
-  <si>
-    <t>2020_10_05_000002_create_jobs_table.php</t>
-  </si>
-  <si>
-    <t>2020_10_05_000003_create_media_table.php</t>
-  </si>
-  <si>
-    <t>2020_10_05_000004_create_user_logins_table.php</t>
-  </si>
-  <si>
-    <t>2020_10_05_000005_create_items_table.php</t>
-  </si>
-  <si>
-    <t>2020_10_05_000006_create_item_groups_table.php</t>
-  </si>
-  <si>
-    <t>2020_10_05_000007_create_menus_table.php</t>
-  </si>
-  <si>
-    <t>2020_10_05_000008_create_price_lists_table.php</t>
-  </si>
-  <si>
-    <t>2020_10_05_000009_create_prices_table.php</t>
-  </si>
-  <si>
-    <t>2020_10_05_000010_create_taxes_table.php</t>
-  </si>
-  <si>
-    <t>2020_10_05_000011_create_kitchens_table.php</t>
-  </si>
-  <si>
-    <t>2020_10_05_000012_create_kitchen_items_table.php</t>
-  </si>
-  <si>
-    <t>2020_10_05_000013_create_kitchen_statuses_table.php</t>
-  </si>
-  <si>
-    <t>2020_10_05_000014_create_customers_table.php</t>
-  </si>
-  <si>
-    <t>2020_10_05_000015_create_seatings_table.php</t>
-  </si>
-  <si>
-    <t>2020_10_05_000016_create_tokens_table.php</t>
-  </si>
-  <si>
-    <t>2020_10_05_000017_create_token_items_table.php</t>
-  </si>
-  <si>
-    <t>2020_10_05_000018_create_bills_table.php</t>
-  </si>
-  <si>
-    <t>2020_10_05_000019_create_payments_table.php</t>
+    <t>2020_11_06_000001_update_users_table.php</t>
+  </si>
+  <si>
+    <t>2020_11_06_000002_create_jobs_table.php</t>
+  </si>
+  <si>
+    <t>2020_11_06_000003_create_media_table.php</t>
+  </si>
+  <si>
+    <t>2020_11_06_000004_create_user_logins_table.php</t>
+  </si>
+  <si>
+    <t>2020_11_06_000005_create_items_table.php</t>
+  </si>
+  <si>
+    <t>2020_11_06_000006_create_item_groups_table.php</t>
+  </si>
+  <si>
+    <t>2020_11_06_000007_create_menus_table.php</t>
+  </si>
+  <si>
+    <t>2020_11_06_000008_create_price_lists_table.php</t>
+  </si>
+  <si>
+    <t>2020_11_06_000009_create_prices_table.php</t>
+  </si>
+  <si>
+    <t>2020_11_06_000010_create_taxes_table.php</t>
+  </si>
+  <si>
+    <t>2020_11_06_000011_create_kitchens_table.php</t>
+  </si>
+  <si>
+    <t>2020_11_06_000012_create_kitchen_items_table.php</t>
+  </si>
+  <si>
+    <t>2020_11_06_000013_create_kitchen_statuses_table.php</t>
+  </si>
+  <si>
+    <t>2020_11_06_000014_create_customers_table.php</t>
+  </si>
+  <si>
+    <t>2020_11_06_000015_create_seatings_table.php</t>
+  </si>
+  <si>
+    <t>2020_11_06_000016_create_tokens_table.php</t>
+  </si>
+  <si>
+    <t>2020_11_06_000017_create_token_items_table.php</t>
+  </si>
+  <si>
+    <t>2020_11_06_000018_create_bills_table.php</t>
+  </si>
+  <si>
+    <t>2020_11_06_000019_create_payments_table.php</t>
+  </si>
+  <si>
+    <t>2020_11_06_000020_create_masters_table.php</t>
+  </si>
+  <si>
+    <t>2020_11_06_000021_create_remote_items_table.php</t>
   </si>
 </sst>
 </file>
@@ -281,15 +287,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F20" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
-  <autoFilter ref="A1:F20"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F22" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="A1:F22"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Files" dataDxfId="1"/>
     <tableColumn id="2" name="Name" dataDxfId="5">
       <calculatedColumnFormula>MID(Table1[[#This Row],[Files]],18,LEN(Table1[[#This Row],[Files]]))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="3" name="Date" dataDxfId="0">
-      <calculatedColumnFormula>"2020_11_06_"</calculatedColumnFormula>
+      <calculatedColumnFormula>"2021_02_08_"</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" name="Seq" dataDxfId="4">
       <calculatedColumnFormula>REPT("0",6-LEN(MATCH(Table1[[#This Row],[Name]],Table1[Name],0)))&amp;MATCH(Table1[[#This Row],[Name]],Table1[Name],0)</calculatedColumnFormula>
@@ -568,10 +574,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F20"/>
+      <selection activeCell="F2" sqref="F2:F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -612,8 +618,8 @@
         <v>_update_users_table.php</v>
       </c>
       <c r="C2" s="1" t="str">
-        <f t="shared" ref="C2:C20" si="0">"2020_11_06_"</f>
-        <v>2020_11_06_</v>
+        <f t="shared" ref="C2:C22" si="0">"2021_02_08_"</f>
+        <v>2021_02_08_</v>
       </c>
       <c r="D2" s="1" t="str">
         <f>REPT("0",6-LEN(MATCH(Table1[[#This Row],[Name]],Table1[Name],0)))&amp;MATCH(Table1[[#This Row],[Name]],Table1[Name],0)</f>
@@ -621,11 +627,11 @@
       </c>
       <c r="E2" s="2" t="str">
         <f>Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Seq]]&amp;Table1[[#This Row],[Name]]</f>
-        <v>2020_11_06_000001_update_users_table.php</v>
+        <v>2021_02_08_000001_update_users_table.php</v>
       </c>
       <c r="F2" s="2" t="str">
         <f>"ren "&amp;Table1[[#This Row],[Files]]&amp;" "&amp;Table1[[#This Row],[Replace]]&amp;";"</f>
-        <v>ren 2020_10_05_000001_update_users_table.php 2020_11_06_000001_update_users_table.php;</v>
+        <v>ren 2020_11_06_000001_update_users_table.php 2021_02_08_000001_update_users_table.php;</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -638,7 +644,7 @@
       </c>
       <c r="C3" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>2020_11_06_</v>
+        <v>2021_02_08_</v>
       </c>
       <c r="D3" s="4" t="str">
         <f>REPT("0",6-LEN(MATCH(Table1[[#This Row],[Name]],Table1[Name],0)))&amp;MATCH(Table1[[#This Row],[Name]],Table1[Name],0)</f>
@@ -646,11 +652,11 @@
       </c>
       <c r="E3" s="4" t="str">
         <f>Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Seq]]&amp;Table1[[#This Row],[Name]]</f>
-        <v>2020_11_06_000002_create_jobs_table.php</v>
+        <v>2021_02_08_000002_create_jobs_table.php</v>
       </c>
       <c r="F3" s="4" t="str">
         <f>"ren "&amp;Table1[[#This Row],[Files]]&amp;" "&amp;Table1[[#This Row],[Replace]]&amp;";"</f>
-        <v>ren 2020_10_05_000002_create_jobs_table.php 2020_11_06_000002_create_jobs_table.php;</v>
+        <v>ren 2020_11_06_000002_create_jobs_table.php 2021_02_08_000002_create_jobs_table.php;</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -663,7 +669,7 @@
       </c>
       <c r="C4" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>2020_11_06_</v>
+        <v>2021_02_08_</v>
       </c>
       <c r="D4" s="1" t="str">
         <f>REPT("0",6-LEN(MATCH(Table1[[#This Row],[Name]],Table1[Name],0)))&amp;MATCH(Table1[[#This Row],[Name]],Table1[Name],0)</f>
@@ -671,24 +677,24 @@
       </c>
       <c r="E4" s="2" t="str">
         <f>Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Seq]]&amp;Table1[[#This Row],[Name]]</f>
-        <v>2020_11_06_000003_create_media_table.php</v>
+        <v>2021_02_08_000003_create_media_table.php</v>
       </c>
       <c r="F4" s="2" t="str">
         <f>"ren "&amp;Table1[[#This Row],[Files]]&amp;" "&amp;Table1[[#This Row],[Replace]]&amp;";"</f>
-        <v>ren 2020_10_05_000003_create_media_table.php 2020_11_06_000003_create_media_table.php;</v>
+        <v>ren 2020_11_06_000003_create_media_table.php 2021_02_08_000003_create_media_table.php;</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="B5" s="1" t="str">
         <f>MID(Table1[[#This Row],[Files]],18,LEN(Table1[[#This Row],[Files]]))</f>
-        <v>_create_user_logins_table.php</v>
+        <v>_create_masters_table.php</v>
       </c>
       <c r="C5" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>2020_11_06_</v>
+        <v>2021_02_08_</v>
       </c>
       <c r="D5" s="1" t="str">
         <f>REPT("0",6-LEN(MATCH(Table1[[#This Row],[Name]],Table1[Name],0)))&amp;MATCH(Table1[[#This Row],[Name]],Table1[Name],0)</f>
@@ -696,24 +702,24 @@
       </c>
       <c r="E5" s="2" t="str">
         <f>Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Seq]]&amp;Table1[[#This Row],[Name]]</f>
-        <v>2020_11_06_000004_create_user_logins_table.php</v>
+        <v>2021_02_08_000004_create_masters_table.php</v>
       </c>
       <c r="F5" s="2" t="str">
         <f>"ren "&amp;Table1[[#This Row],[Files]]&amp;" "&amp;Table1[[#This Row],[Replace]]&amp;";"</f>
-        <v>ren 2020_10_05_000004_create_user_logins_table.php 2020_11_06_000004_create_user_logins_table.php;</v>
+        <v>ren 2020_11_06_000020_create_masters_table.php 2021_02_08_000004_create_masters_table.php;</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B6" s="1" t="str">
         <f>MID(Table1[[#This Row],[Files]],18,LEN(Table1[[#This Row],[Files]]))</f>
-        <v>_create_items_table.php</v>
+        <v>_create_user_logins_table.php</v>
       </c>
       <c r="C6" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>2020_11_06_</v>
+        <v>2021_02_08_</v>
       </c>
       <c r="D6" s="1" t="str">
         <f>REPT("0",6-LEN(MATCH(Table1[[#This Row],[Name]],Table1[Name],0)))&amp;MATCH(Table1[[#This Row],[Name]],Table1[Name],0)</f>
@@ -721,24 +727,24 @@
       </c>
       <c r="E6" s="2" t="str">
         <f>Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Seq]]&amp;Table1[[#This Row],[Name]]</f>
-        <v>2020_11_06_000005_create_items_table.php</v>
+        <v>2021_02_08_000005_create_user_logins_table.php</v>
       </c>
       <c r="F6" s="2" t="str">
         <f>"ren "&amp;Table1[[#This Row],[Files]]&amp;" "&amp;Table1[[#This Row],[Replace]]&amp;";"</f>
-        <v>ren 2020_10_05_000005_create_items_table.php 2020_11_06_000005_create_items_table.php;</v>
+        <v>ren 2020_11_06_000004_create_user_logins_table.php 2021_02_08_000005_create_user_logins_table.php;</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B7" s="1" t="str">
         <f>MID(Table1[[#This Row],[Files]],18,LEN(Table1[[#This Row],[Files]]))</f>
-        <v>_create_item_groups_table.php</v>
+        <v>_create_items_table.php</v>
       </c>
       <c r="C7" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>2020_11_06_</v>
+        <v>2021_02_08_</v>
       </c>
       <c r="D7" s="1" t="str">
         <f>REPT("0",6-LEN(MATCH(Table1[[#This Row],[Name]],Table1[Name],0)))&amp;MATCH(Table1[[#This Row],[Name]],Table1[Name],0)</f>
@@ -746,24 +752,24 @@
       </c>
       <c r="E7" s="2" t="str">
         <f>Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Seq]]&amp;Table1[[#This Row],[Name]]</f>
-        <v>2020_11_06_000006_create_item_groups_table.php</v>
+        <v>2021_02_08_000006_create_items_table.php</v>
       </c>
       <c r="F7" s="2" t="str">
         <f>"ren "&amp;Table1[[#This Row],[Files]]&amp;" "&amp;Table1[[#This Row],[Replace]]&amp;";"</f>
-        <v>ren 2020_10_05_000006_create_item_groups_table.php 2020_11_06_000006_create_item_groups_table.php;</v>
+        <v>ren 2020_11_06_000005_create_items_table.php 2021_02_08_000006_create_items_table.php;</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B8" s="1" t="str">
         <f>MID(Table1[[#This Row],[Files]],18,LEN(Table1[[#This Row],[Files]]))</f>
-        <v>_create_menus_table.php</v>
+        <v>_create_item_groups_table.php</v>
       </c>
       <c r="C8" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>2020_11_06_</v>
+        <v>2021_02_08_</v>
       </c>
       <c r="D8" s="1" t="str">
         <f>REPT("0",6-LEN(MATCH(Table1[[#This Row],[Name]],Table1[Name],0)))&amp;MATCH(Table1[[#This Row],[Name]],Table1[Name],0)</f>
@@ -771,24 +777,24 @@
       </c>
       <c r="E8" s="2" t="str">
         <f>Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Seq]]&amp;Table1[[#This Row],[Name]]</f>
-        <v>2020_11_06_000007_create_menus_table.php</v>
+        <v>2021_02_08_000007_create_item_groups_table.php</v>
       </c>
       <c r="F8" s="2" t="str">
         <f>"ren "&amp;Table1[[#This Row],[Files]]&amp;" "&amp;Table1[[#This Row],[Replace]]&amp;";"</f>
-        <v>ren 2020_10_05_000007_create_menus_table.php 2020_11_06_000007_create_menus_table.php;</v>
+        <v>ren 2020_11_06_000006_create_item_groups_table.php 2021_02_08_000007_create_item_groups_table.php;</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B9" s="1" t="str">
         <f>MID(Table1[[#This Row],[Files]],18,LEN(Table1[[#This Row],[Files]]))</f>
-        <v>_create_price_lists_table.php</v>
+        <v>_create_menus_table.php</v>
       </c>
       <c r="C9" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>2020_11_06_</v>
+        <v>2021_02_08_</v>
       </c>
       <c r="D9" s="1" t="str">
         <f>REPT("0",6-LEN(MATCH(Table1[[#This Row],[Name]],Table1[Name],0)))&amp;MATCH(Table1[[#This Row],[Name]],Table1[Name],0)</f>
@@ -796,24 +802,24 @@
       </c>
       <c r="E9" s="2" t="str">
         <f>Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Seq]]&amp;Table1[[#This Row],[Name]]</f>
-        <v>2020_11_06_000008_create_price_lists_table.php</v>
+        <v>2021_02_08_000008_create_menus_table.php</v>
       </c>
       <c r="F9" s="2" t="str">
         <f>"ren "&amp;Table1[[#This Row],[Files]]&amp;" "&amp;Table1[[#This Row],[Replace]]&amp;";"</f>
-        <v>ren 2020_10_05_000008_create_price_lists_table.php 2020_11_06_000008_create_price_lists_table.php;</v>
+        <v>ren 2020_11_06_000007_create_menus_table.php 2021_02_08_000008_create_menus_table.php;</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B10" s="1" t="str">
         <f>MID(Table1[[#This Row],[Files]],18,LEN(Table1[[#This Row],[Files]]))</f>
-        <v>_create_prices_table.php</v>
+        <v>_create_price_lists_table.php</v>
       </c>
       <c r="C10" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>2020_11_06_</v>
+        <v>2021_02_08_</v>
       </c>
       <c r="D10" s="1" t="str">
         <f>REPT("0",6-LEN(MATCH(Table1[[#This Row],[Name]],Table1[Name],0)))&amp;MATCH(Table1[[#This Row],[Name]],Table1[Name],0)</f>
@@ -821,24 +827,24 @@
       </c>
       <c r="E10" s="2" t="str">
         <f>Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Seq]]&amp;Table1[[#This Row],[Name]]</f>
-        <v>2020_11_06_000009_create_prices_table.php</v>
+        <v>2021_02_08_000009_create_price_lists_table.php</v>
       </c>
       <c r="F10" s="2" t="str">
         <f>"ren "&amp;Table1[[#This Row],[Files]]&amp;" "&amp;Table1[[#This Row],[Replace]]&amp;";"</f>
-        <v>ren 2020_10_05_000009_create_prices_table.php 2020_11_06_000009_create_prices_table.php;</v>
+        <v>ren 2020_11_06_000008_create_price_lists_table.php 2021_02_08_000009_create_price_lists_table.php;</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B11" s="1" t="str">
         <f>MID(Table1[[#This Row],[Files]],18,LEN(Table1[[#This Row],[Files]]))</f>
-        <v>_create_taxes_table.php</v>
+        <v>_create_prices_table.php</v>
       </c>
       <c r="C11" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>2020_11_06_</v>
+        <v>2021_02_08_</v>
       </c>
       <c r="D11" s="1" t="str">
         <f>REPT("0",6-LEN(MATCH(Table1[[#This Row],[Name]],Table1[Name],0)))&amp;MATCH(Table1[[#This Row],[Name]],Table1[Name],0)</f>
@@ -846,24 +852,24 @@
       </c>
       <c r="E11" s="2" t="str">
         <f>Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Seq]]&amp;Table1[[#This Row],[Name]]</f>
-        <v>2020_11_06_000010_create_taxes_table.php</v>
+        <v>2021_02_08_000010_create_prices_table.php</v>
       </c>
       <c r="F11" s="2" t="str">
         <f>"ren "&amp;Table1[[#This Row],[Files]]&amp;" "&amp;Table1[[#This Row],[Replace]]&amp;";"</f>
-        <v>ren 2020_10_05_000010_create_taxes_table.php 2020_11_06_000010_create_taxes_table.php;</v>
+        <v>ren 2020_11_06_000009_create_prices_table.php 2021_02_08_000010_create_prices_table.php;</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B12" s="4" t="str">
         <f>MID(Table1[[#This Row],[Files]],18,LEN(Table1[[#This Row],[Files]]))</f>
-        <v>_create_kitchens_table.php</v>
+        <v>_create_taxes_table.php</v>
       </c>
       <c r="C12" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>2020_11_06_</v>
+        <v>2021_02_08_</v>
       </c>
       <c r="D12" s="4" t="str">
         <f>REPT("0",6-LEN(MATCH(Table1[[#This Row],[Name]],Table1[Name],0)))&amp;MATCH(Table1[[#This Row],[Name]],Table1[Name],0)</f>
@@ -871,24 +877,24 @@
       </c>
       <c r="E12" s="4" t="str">
         <f>Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Seq]]&amp;Table1[[#This Row],[Name]]</f>
-        <v>2020_11_06_000011_create_kitchens_table.php</v>
+        <v>2021_02_08_000011_create_taxes_table.php</v>
       </c>
       <c r="F12" s="4" t="str">
         <f>"ren "&amp;Table1[[#This Row],[Files]]&amp;" "&amp;Table1[[#This Row],[Replace]]&amp;";"</f>
-        <v>ren 2020_10_05_000011_create_kitchens_table.php 2020_11_06_000011_create_kitchens_table.php;</v>
+        <v>ren 2020_11_06_000010_create_taxes_table.php 2021_02_08_000011_create_taxes_table.php;</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B13" s="1" t="str">
         <f>MID(Table1[[#This Row],[Files]],18,LEN(Table1[[#This Row],[Files]]))</f>
-        <v>_create_kitchen_items_table.php</v>
+        <v>_create_kitchens_table.php</v>
       </c>
       <c r="C13" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>2020_11_06_</v>
+        <v>2021_02_08_</v>
       </c>
       <c r="D13" s="1" t="str">
         <f>REPT("0",6-LEN(MATCH(Table1[[#This Row],[Name]],Table1[Name],0)))&amp;MATCH(Table1[[#This Row],[Name]],Table1[Name],0)</f>
@@ -896,24 +902,24 @@
       </c>
       <c r="E13" s="2" t="str">
         <f>Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Seq]]&amp;Table1[[#This Row],[Name]]</f>
-        <v>2020_11_06_000012_create_kitchen_items_table.php</v>
+        <v>2021_02_08_000012_create_kitchens_table.php</v>
       </c>
       <c r="F13" s="2" t="str">
         <f>"ren "&amp;Table1[[#This Row],[Files]]&amp;" "&amp;Table1[[#This Row],[Replace]]&amp;";"</f>
-        <v>ren 2020_10_05_000012_create_kitchen_items_table.php 2020_11_06_000012_create_kitchen_items_table.php;</v>
+        <v>ren 2020_11_06_000011_create_kitchens_table.php 2021_02_08_000012_create_kitchens_table.php;</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B14" s="1" t="str">
         <f>MID(Table1[[#This Row],[Files]],18,LEN(Table1[[#This Row],[Files]]))</f>
-        <v>_create_kitchen_statuses_table.php</v>
+        <v>_create_kitchen_items_table.php</v>
       </c>
       <c r="C14" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>2020_11_06_</v>
+        <v>2021_02_08_</v>
       </c>
       <c r="D14" s="1" t="str">
         <f>REPT("0",6-LEN(MATCH(Table1[[#This Row],[Name]],Table1[Name],0)))&amp;MATCH(Table1[[#This Row],[Name]],Table1[Name],0)</f>
@@ -921,24 +927,24 @@
       </c>
       <c r="E14" s="2" t="str">
         <f>Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Seq]]&amp;Table1[[#This Row],[Name]]</f>
-        <v>2020_11_06_000013_create_kitchen_statuses_table.php</v>
+        <v>2021_02_08_000013_create_kitchen_items_table.php</v>
       </c>
       <c r="F14" s="2" t="str">
         <f>"ren "&amp;Table1[[#This Row],[Files]]&amp;" "&amp;Table1[[#This Row],[Replace]]&amp;";"</f>
-        <v>ren 2020_10_05_000013_create_kitchen_statuses_table.php 2020_11_06_000013_create_kitchen_statuses_table.php;</v>
+        <v>ren 2020_11_06_000012_create_kitchen_items_table.php 2021_02_08_000013_create_kitchen_items_table.php;</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B15" s="1" t="str">
         <f>MID(Table1[[#This Row],[Files]],18,LEN(Table1[[#This Row],[Files]]))</f>
-        <v>_create_customers_table.php</v>
+        <v>_create_kitchen_statuses_table.php</v>
       </c>
       <c r="C15" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>2020_11_06_</v>
+        <v>2021_02_08_</v>
       </c>
       <c r="D15" s="1" t="str">
         <f>REPT("0",6-LEN(MATCH(Table1[[#This Row],[Name]],Table1[Name],0)))&amp;MATCH(Table1[[#This Row],[Name]],Table1[Name],0)</f>
@@ -946,24 +952,24 @@
       </c>
       <c r="E15" s="2" t="str">
         <f>Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Seq]]&amp;Table1[[#This Row],[Name]]</f>
-        <v>2020_11_06_000014_create_customers_table.php</v>
+        <v>2021_02_08_000014_create_kitchen_statuses_table.php</v>
       </c>
       <c r="F15" s="2" t="str">
         <f>"ren "&amp;Table1[[#This Row],[Files]]&amp;" "&amp;Table1[[#This Row],[Replace]]&amp;";"</f>
-        <v>ren 2020_10_05_000014_create_customers_table.php 2020_11_06_000014_create_customers_table.php;</v>
+        <v>ren 2020_11_06_000013_create_kitchen_statuses_table.php 2021_02_08_000014_create_kitchen_statuses_table.php;</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B16" s="1" t="str">
         <f>MID(Table1[[#This Row],[Files]],18,LEN(Table1[[#This Row],[Files]]))</f>
-        <v>_create_seatings_table.php</v>
+        <v>_create_customers_table.php</v>
       </c>
       <c r="C16" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>2020_11_06_</v>
+        <v>2021_02_08_</v>
       </c>
       <c r="D16" s="1" t="str">
         <f>REPT("0",6-LEN(MATCH(Table1[[#This Row],[Name]],Table1[Name],0)))&amp;MATCH(Table1[[#This Row],[Name]],Table1[Name],0)</f>
@@ -971,24 +977,24 @@
       </c>
       <c r="E16" s="2" t="str">
         <f>Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Seq]]&amp;Table1[[#This Row],[Name]]</f>
-        <v>2020_11_06_000015_create_seatings_table.php</v>
+        <v>2021_02_08_000015_create_customers_table.php</v>
       </c>
       <c r="F16" s="2" t="str">
         <f>"ren "&amp;Table1[[#This Row],[Files]]&amp;" "&amp;Table1[[#This Row],[Replace]]&amp;";"</f>
-        <v>ren 2020_10_05_000015_create_seatings_table.php 2020_11_06_000015_create_seatings_table.php;</v>
+        <v>ren 2020_11_06_000014_create_customers_table.php 2021_02_08_000015_create_customers_table.php;</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B17" s="1" t="str">
         <f>MID(Table1[[#This Row],[Files]],18,LEN(Table1[[#This Row],[Files]]))</f>
-        <v>_create_tokens_table.php</v>
+        <v>_create_seatings_table.php</v>
       </c>
       <c r="C17" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>2020_11_06_</v>
+        <v>2021_02_08_</v>
       </c>
       <c r="D17" s="1" t="str">
         <f>REPT("0",6-LEN(MATCH(Table1[[#This Row],[Name]],Table1[Name],0)))&amp;MATCH(Table1[[#This Row],[Name]],Table1[Name],0)</f>
@@ -996,24 +1002,24 @@
       </c>
       <c r="E17" s="2" t="str">
         <f>Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Seq]]&amp;Table1[[#This Row],[Name]]</f>
-        <v>2020_11_06_000016_create_tokens_table.php</v>
+        <v>2021_02_08_000016_create_seatings_table.php</v>
       </c>
       <c r="F17" s="2" t="str">
         <f>"ren "&amp;Table1[[#This Row],[Files]]&amp;" "&amp;Table1[[#This Row],[Replace]]&amp;";"</f>
-        <v>ren 2020_10_05_000016_create_tokens_table.php 2020_11_06_000016_create_tokens_table.php;</v>
+        <v>ren 2020_11_06_000015_create_seatings_table.php 2021_02_08_000016_create_seatings_table.php;</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B18" s="1" t="str">
         <f>MID(Table1[[#This Row],[Files]],18,LEN(Table1[[#This Row],[Files]]))</f>
-        <v>_create_token_items_table.php</v>
+        <v>_create_tokens_table.php</v>
       </c>
       <c r="C18" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>2020_11_06_</v>
+        <v>2021_02_08_</v>
       </c>
       <c r="D18" s="1" t="str">
         <f>REPT("0",6-LEN(MATCH(Table1[[#This Row],[Name]],Table1[Name],0)))&amp;MATCH(Table1[[#This Row],[Name]],Table1[Name],0)</f>
@@ -1021,24 +1027,24 @@
       </c>
       <c r="E18" s="2" t="str">
         <f>Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Seq]]&amp;Table1[[#This Row],[Name]]</f>
-        <v>2020_11_06_000017_create_token_items_table.php</v>
+        <v>2021_02_08_000017_create_tokens_table.php</v>
       </c>
       <c r="F18" s="2" t="str">
         <f>"ren "&amp;Table1[[#This Row],[Files]]&amp;" "&amp;Table1[[#This Row],[Replace]]&amp;";"</f>
-        <v>ren 2020_10_05_000017_create_token_items_table.php 2020_11_06_000017_create_token_items_table.php;</v>
+        <v>ren 2020_11_06_000016_create_tokens_table.php 2021_02_08_000017_create_tokens_table.php;</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B19" s="4" t="str">
         <f>MID(Table1[[#This Row],[Files]],18,LEN(Table1[[#This Row],[Files]]))</f>
-        <v>_create_bills_table.php</v>
+        <v>_create_token_items_table.php</v>
       </c>
       <c r="C19" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>2020_11_06_</v>
+        <v>2021_02_08_</v>
       </c>
       <c r="D19" s="4" t="str">
         <f>REPT("0",6-LEN(MATCH(Table1[[#This Row],[Name]],Table1[Name],0)))&amp;MATCH(Table1[[#This Row],[Name]],Table1[Name],0)</f>
@@ -1046,36 +1052,86 @@
       </c>
       <c r="E19" s="4" t="str">
         <f>Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Seq]]&amp;Table1[[#This Row],[Name]]</f>
-        <v>2020_11_06_000018_create_bills_table.php</v>
+        <v>2021_02_08_000018_create_token_items_table.php</v>
       </c>
       <c r="F19" s="4" t="str">
         <f>"ren "&amp;Table1[[#This Row],[Files]]&amp;" "&amp;Table1[[#This Row],[Replace]]&amp;";"</f>
-        <v>ren 2020_10_05_000018_create_bills_table.php 2020_11_06_000018_create_bills_table.php;</v>
+        <v>ren 2020_11_06_000017_create_token_items_table.php 2021_02_08_000018_create_token_items_table.php;</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20" s="4" t="str">
+        <f>MID(Table1[[#This Row],[Files]],18,LEN(Table1[[#This Row],[Files]]))</f>
+        <v>_create_bills_table.php</v>
+      </c>
+      <c r="C20" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>2021_02_08_</v>
+      </c>
+      <c r="D20" s="4" t="str">
+        <f>REPT("0",6-LEN(MATCH(Table1[[#This Row],[Name]],Table1[Name],0)))&amp;MATCH(Table1[[#This Row],[Name]],Table1[Name],0)</f>
+        <v>000019</v>
+      </c>
+      <c r="E20" s="4" t="str">
+        <f>Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Seq]]&amp;Table1[[#This Row],[Name]]</f>
+        <v>2021_02_08_000019_create_bills_table.php</v>
+      </c>
+      <c r="F20" s="4" t="str">
+        <f>"ren "&amp;Table1[[#This Row],[Files]]&amp;" "&amp;Table1[[#This Row],[Replace]]&amp;";"</f>
+        <v>ren 2020_11_06_000018_create_bills_table.php 2021_02_08_000019_create_bills_table.php;</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B20" s="4" t="str">
+      <c r="B21" s="4" t="str">
         <f>MID(Table1[[#This Row],[Files]],18,LEN(Table1[[#This Row],[Files]]))</f>
         <v>_create_payments_table.php</v>
       </c>
-      <c r="C20" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v>2020_11_06_</v>
-      </c>
-      <c r="D20" s="4" t="str">
-        <f>REPT("0",6-LEN(MATCH(Table1[[#This Row],[Name]],Table1[Name],0)))&amp;MATCH(Table1[[#This Row],[Name]],Table1[Name],0)</f>
-        <v>000019</v>
-      </c>
-      <c r="E20" s="4" t="str">
-        <f>Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Seq]]&amp;Table1[[#This Row],[Name]]</f>
-        <v>2020_11_06_000019_create_payments_table.php</v>
-      </c>
-      <c r="F20" s="4" t="str">
-        <f>"ren "&amp;Table1[[#This Row],[Files]]&amp;" "&amp;Table1[[#This Row],[Replace]]&amp;";"</f>
-        <v>ren 2020_10_05_000019_create_payments_table.php 2020_11_06_000019_create_payments_table.php;</v>
+      <c r="C21" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>2021_02_08_</v>
+      </c>
+      <c r="D21" s="4" t="str">
+        <f>REPT("0",6-LEN(MATCH(Table1[[#This Row],[Name]],Table1[Name],0)))&amp;MATCH(Table1[[#This Row],[Name]],Table1[Name],0)</f>
+        <v>000020</v>
+      </c>
+      <c r="E21" s="4" t="str">
+        <f>Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Seq]]&amp;Table1[[#This Row],[Name]]</f>
+        <v>2021_02_08_000020_create_payments_table.php</v>
+      </c>
+      <c r="F21" s="4" t="str">
+        <f>"ren "&amp;Table1[[#This Row],[Files]]&amp;" "&amp;Table1[[#This Row],[Replace]]&amp;";"</f>
+        <v>ren 2020_11_06_000019_create_payments_table.php 2021_02_08_000020_create_payments_table.php;</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B22" s="4" t="str">
+        <f>MID(Table1[[#This Row],[Files]],18,LEN(Table1[[#This Row],[Files]]))</f>
+        <v>_create_remote_items_table.php</v>
+      </c>
+      <c r="C22" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>2021_02_08_</v>
+      </c>
+      <c r="D22" s="4" t="str">
+        <f>REPT("0",6-LEN(MATCH(Table1[[#This Row],[Name]],Table1[Name],0)))&amp;MATCH(Table1[[#This Row],[Name]],Table1[Name],0)</f>
+        <v>000021</v>
+      </c>
+      <c r="E22" s="4" t="str">
+        <f>Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Seq]]&amp;Table1[[#This Row],[Name]]</f>
+        <v>2021_02_08_000021_create_remote_items_table.php</v>
+      </c>
+      <c r="F22" s="4" t="str">
+        <f>"ren "&amp;Table1[[#This Row],[Files]]&amp;" "&amp;Table1[[#This Row],[Replace]]&amp;";"</f>
+        <v>ren 2020_11_06_000021_create_remote_items_table.php 2021_02_08_000021_create_remote_items_table.php;</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Master changed as settings
</commit_message>
<xml_diff>
--- a/MigrationRenamer.xlsx
+++ b/MigrationRenamer.xlsx
@@ -44,67 +44,67 @@
     <t>CMD</t>
   </si>
   <si>
-    <t>2020_11_06_000001_update_users_table.php</t>
-  </si>
-  <si>
-    <t>2020_11_06_000002_create_jobs_table.php</t>
-  </si>
-  <si>
-    <t>2020_11_06_000003_create_media_table.php</t>
-  </si>
-  <si>
-    <t>2020_11_06_000004_create_user_logins_table.php</t>
-  </si>
-  <si>
-    <t>2020_11_06_000005_create_items_table.php</t>
-  </si>
-  <si>
-    <t>2020_11_06_000006_create_item_groups_table.php</t>
-  </si>
-  <si>
-    <t>2020_11_06_000007_create_menus_table.php</t>
-  </si>
-  <si>
-    <t>2020_11_06_000008_create_price_lists_table.php</t>
-  </si>
-  <si>
-    <t>2020_11_06_000009_create_prices_table.php</t>
-  </si>
-  <si>
-    <t>2020_11_06_000010_create_taxes_table.php</t>
-  </si>
-  <si>
-    <t>2020_11_06_000011_create_kitchens_table.php</t>
-  </si>
-  <si>
-    <t>2020_11_06_000012_create_kitchen_items_table.php</t>
-  </si>
-  <si>
-    <t>2020_11_06_000013_create_kitchen_statuses_table.php</t>
-  </si>
-  <si>
-    <t>2020_11_06_000014_create_customers_table.php</t>
-  </si>
-  <si>
-    <t>2020_11_06_000015_create_seatings_table.php</t>
-  </si>
-  <si>
-    <t>2020_11_06_000016_create_tokens_table.php</t>
-  </si>
-  <si>
-    <t>2020_11_06_000017_create_token_items_table.php</t>
-  </si>
-  <si>
-    <t>2020_11_06_000018_create_bills_table.php</t>
-  </si>
-  <si>
-    <t>2020_11_06_000019_create_payments_table.php</t>
-  </si>
-  <si>
-    <t>2020_11_06_000020_create_masters_table.php</t>
-  </si>
-  <si>
-    <t>2020_11_06_000021_create_remote_items_table.php</t>
+    <t>2021_03_25_000001_update_users_table.php</t>
+  </si>
+  <si>
+    <t>2021_03_25_000002_create_jobs_table.php</t>
+  </si>
+  <si>
+    <t>2021_03_25_000004_create_masters_table.php</t>
+  </si>
+  <si>
+    <t>2021_03_25_000005_create_user_logins_table.php</t>
+  </si>
+  <si>
+    <t>2021_03_25_000006_create_items_table.php</t>
+  </si>
+  <si>
+    <t>2021_03_25_000007_create_item_groups_table.php</t>
+  </si>
+  <si>
+    <t>2021_03_25_000008_create_menus_table.php</t>
+  </si>
+  <si>
+    <t>2021_03_25_000009_create_price_lists_table.php</t>
+  </si>
+  <si>
+    <t>2021_03_25_000010_create_prices_table.php</t>
+  </si>
+  <si>
+    <t>2021_03_25_000011_create_taxes_table.php</t>
+  </si>
+  <si>
+    <t>2021_03_25_000012_create_kitchens_table.php</t>
+  </si>
+  <si>
+    <t>2021_03_25_000013_create_kitchen_items_table.php</t>
+  </si>
+  <si>
+    <t>2021_03_25_000014_create_kitchen_statuses_table.php</t>
+  </si>
+  <si>
+    <t>2021_03_25_000015_create_customers_table.php</t>
+  </si>
+  <si>
+    <t>2021_03_25_000016_create_seatings_table.php</t>
+  </si>
+  <si>
+    <t>2021_03_25_000017_create_tokens_table.php</t>
+  </si>
+  <si>
+    <t>2021_03_25_000018_create_token_items_table.php</t>
+  </si>
+  <si>
+    <t>2021_03_25_000019_create_bills_table.php</t>
+  </si>
+  <si>
+    <t>2021_03_25_000020_create_payments_table.php</t>
+  </si>
+  <si>
+    <t>2021_03_25_000021_create_remote_table.php</t>
+  </si>
+  <si>
+    <t>2021_03_25_150256_create_settings_table.php</t>
   </si>
 </sst>
 </file>
@@ -190,19 +190,6 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
@@ -273,6 +260,19 @@
         <scheme val="minor"/>
       </font>
     </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -290,20 +290,20 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F22" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
   <autoFilter ref="A1:F22"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="Files" dataDxfId="1"/>
-    <tableColumn id="2" name="Name" dataDxfId="5">
+    <tableColumn id="1" name="Files" dataDxfId="5"/>
+    <tableColumn id="2" name="Name" dataDxfId="4">
       <calculatedColumnFormula>MID(Table1[[#This Row],[Files]],18,LEN(Table1[[#This Row],[Files]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Date" dataDxfId="0">
-      <calculatedColumnFormula>"2021_02_08_"</calculatedColumnFormula>
+    <tableColumn id="3" name="Date" dataDxfId="3">
+      <calculatedColumnFormula>"2021_03_25_"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Seq" dataDxfId="4">
+    <tableColumn id="4" name="Seq" dataDxfId="2">
       <calculatedColumnFormula>REPT("0",6-LEN(MATCH(Table1[[#This Row],[Name]],Table1[Name],0)))&amp;MATCH(Table1[[#This Row],[Name]],Table1[Name],0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="Replace" dataDxfId="3">
+    <tableColumn id="5" name="Replace" dataDxfId="1">
       <calculatedColumnFormula>Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Seq]]&amp;Table1[[#This Row],[Name]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="CMD" dataDxfId="2">
+    <tableColumn id="6" name="CMD" dataDxfId="0">
       <calculatedColumnFormula>"ren "&amp;Table1[[#This Row],[Files]]&amp;" "&amp;Table1[[#This Row],[Replace]]&amp;";"</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -576,7 +576,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <selection activeCell="F2" sqref="F2:F22"/>
     </sheetView>
   </sheetViews>
@@ -618,8 +618,8 @@
         <v>_update_users_table.php</v>
       </c>
       <c r="C2" s="1" t="str">
-        <f t="shared" ref="C2:C22" si="0">"2021_02_08_"</f>
-        <v>2021_02_08_</v>
+        <f t="shared" ref="C2:C22" si="0">"2021_03_25_"</f>
+        <v>2021_03_25_</v>
       </c>
       <c r="D2" s="1" t="str">
         <f>REPT("0",6-LEN(MATCH(Table1[[#This Row],[Name]],Table1[Name],0)))&amp;MATCH(Table1[[#This Row],[Name]],Table1[Name],0)</f>
@@ -627,11 +627,11 @@
       </c>
       <c r="E2" s="2" t="str">
         <f>Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Seq]]&amp;Table1[[#This Row],[Name]]</f>
-        <v>2021_02_08_000001_update_users_table.php</v>
+        <v>2021_03_25_000001_update_users_table.php</v>
       </c>
       <c r="F2" s="2" t="str">
         <f>"ren "&amp;Table1[[#This Row],[Files]]&amp;" "&amp;Table1[[#This Row],[Replace]]&amp;";"</f>
-        <v>ren 2020_11_06_000001_update_users_table.php 2021_02_08_000001_update_users_table.php;</v>
+        <v>ren 2021_03_25_000001_update_users_table.php 2021_03_25_000001_update_users_table.php;</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -644,7 +644,7 @@
       </c>
       <c r="C3" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>2021_02_08_</v>
+        <v>2021_03_25_</v>
       </c>
       <c r="D3" s="4" t="str">
         <f>REPT("0",6-LEN(MATCH(Table1[[#This Row],[Name]],Table1[Name],0)))&amp;MATCH(Table1[[#This Row],[Name]],Table1[Name],0)</f>
@@ -652,24 +652,24 @@
       </c>
       <c r="E3" s="4" t="str">
         <f>Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Seq]]&amp;Table1[[#This Row],[Name]]</f>
-        <v>2021_02_08_000002_create_jobs_table.php</v>
+        <v>2021_03_25_000002_create_jobs_table.php</v>
       </c>
       <c r="F3" s="4" t="str">
         <f>"ren "&amp;Table1[[#This Row],[Files]]&amp;" "&amp;Table1[[#This Row],[Replace]]&amp;";"</f>
-        <v>ren 2020_11_06_000002_create_jobs_table.php 2021_02_08_000002_create_jobs_table.php;</v>
+        <v>ren 2021_03_25_000002_create_jobs_table.php 2021_03_25_000002_create_jobs_table.php;</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>8</v>
+      <c r="A4" s="3" t="s">
+        <v>26</v>
       </c>
       <c r="B4" s="1" t="str">
         <f>MID(Table1[[#This Row],[Files]],18,LEN(Table1[[#This Row],[Files]]))</f>
-        <v>_create_media_table.php</v>
+        <v>_create_settings_table.php</v>
       </c>
       <c r="C4" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>2021_02_08_</v>
+        <v>2021_03_25_</v>
       </c>
       <c r="D4" s="1" t="str">
         <f>REPT("0",6-LEN(MATCH(Table1[[#This Row],[Name]],Table1[Name],0)))&amp;MATCH(Table1[[#This Row],[Name]],Table1[Name],0)</f>
@@ -677,16 +677,16 @@
       </c>
       <c r="E4" s="2" t="str">
         <f>Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Seq]]&amp;Table1[[#This Row],[Name]]</f>
-        <v>2021_02_08_000003_create_media_table.php</v>
+        <v>2021_03_25_000003_create_settings_table.php</v>
       </c>
       <c r="F4" s="2" t="str">
         <f>"ren "&amp;Table1[[#This Row],[Files]]&amp;" "&amp;Table1[[#This Row],[Replace]]&amp;";"</f>
-        <v>ren 2020_11_06_000003_create_media_table.php 2021_02_08_000003_create_media_table.php;</v>
+        <v>ren 2021_03_25_150256_create_settings_table.php 2021_03_25_000003_create_settings_table.php;</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="B5" s="1" t="str">
         <f>MID(Table1[[#This Row],[Files]],18,LEN(Table1[[#This Row],[Files]]))</f>
@@ -694,7 +694,7 @@
       </c>
       <c r="C5" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>2021_02_08_</v>
+        <v>2021_03_25_</v>
       </c>
       <c r="D5" s="1" t="str">
         <f>REPT("0",6-LEN(MATCH(Table1[[#This Row],[Name]],Table1[Name],0)))&amp;MATCH(Table1[[#This Row],[Name]],Table1[Name],0)</f>
@@ -702,11 +702,11 @@
       </c>
       <c r="E5" s="2" t="str">
         <f>Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Seq]]&amp;Table1[[#This Row],[Name]]</f>
-        <v>2021_02_08_000004_create_masters_table.php</v>
+        <v>2021_03_25_000004_create_masters_table.php</v>
       </c>
       <c r="F5" s="2" t="str">
         <f>"ren "&amp;Table1[[#This Row],[Files]]&amp;" "&amp;Table1[[#This Row],[Replace]]&amp;";"</f>
-        <v>ren 2020_11_06_000020_create_masters_table.php 2021_02_08_000004_create_masters_table.php;</v>
+        <v>ren 2021_03_25_000004_create_masters_table.php 2021_03_25_000004_create_masters_table.php;</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -719,7 +719,7 @@
       </c>
       <c r="C6" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>2021_02_08_</v>
+        <v>2021_03_25_</v>
       </c>
       <c r="D6" s="1" t="str">
         <f>REPT("0",6-LEN(MATCH(Table1[[#This Row],[Name]],Table1[Name],0)))&amp;MATCH(Table1[[#This Row],[Name]],Table1[Name],0)</f>
@@ -727,11 +727,11 @@
       </c>
       <c r="E6" s="2" t="str">
         <f>Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Seq]]&amp;Table1[[#This Row],[Name]]</f>
-        <v>2021_02_08_000005_create_user_logins_table.php</v>
+        <v>2021_03_25_000005_create_user_logins_table.php</v>
       </c>
       <c r="F6" s="2" t="str">
         <f>"ren "&amp;Table1[[#This Row],[Files]]&amp;" "&amp;Table1[[#This Row],[Replace]]&amp;";"</f>
-        <v>ren 2020_11_06_000004_create_user_logins_table.php 2021_02_08_000005_create_user_logins_table.php;</v>
+        <v>ren 2021_03_25_000005_create_user_logins_table.php 2021_03_25_000005_create_user_logins_table.php;</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -744,7 +744,7 @@
       </c>
       <c r="C7" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>2021_02_08_</v>
+        <v>2021_03_25_</v>
       </c>
       <c r="D7" s="1" t="str">
         <f>REPT("0",6-LEN(MATCH(Table1[[#This Row],[Name]],Table1[Name],0)))&amp;MATCH(Table1[[#This Row],[Name]],Table1[Name],0)</f>
@@ -752,11 +752,11 @@
       </c>
       <c r="E7" s="2" t="str">
         <f>Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Seq]]&amp;Table1[[#This Row],[Name]]</f>
-        <v>2021_02_08_000006_create_items_table.php</v>
+        <v>2021_03_25_000006_create_items_table.php</v>
       </c>
       <c r="F7" s="2" t="str">
         <f>"ren "&amp;Table1[[#This Row],[Files]]&amp;" "&amp;Table1[[#This Row],[Replace]]&amp;";"</f>
-        <v>ren 2020_11_06_000005_create_items_table.php 2021_02_08_000006_create_items_table.php;</v>
+        <v>ren 2021_03_25_000006_create_items_table.php 2021_03_25_000006_create_items_table.php;</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -769,7 +769,7 @@
       </c>
       <c r="C8" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>2021_02_08_</v>
+        <v>2021_03_25_</v>
       </c>
       <c r="D8" s="1" t="str">
         <f>REPT("0",6-LEN(MATCH(Table1[[#This Row],[Name]],Table1[Name],0)))&amp;MATCH(Table1[[#This Row],[Name]],Table1[Name],0)</f>
@@ -777,11 +777,11 @@
       </c>
       <c r="E8" s="2" t="str">
         <f>Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Seq]]&amp;Table1[[#This Row],[Name]]</f>
-        <v>2021_02_08_000007_create_item_groups_table.php</v>
+        <v>2021_03_25_000007_create_item_groups_table.php</v>
       </c>
       <c r="F8" s="2" t="str">
         <f>"ren "&amp;Table1[[#This Row],[Files]]&amp;" "&amp;Table1[[#This Row],[Replace]]&amp;";"</f>
-        <v>ren 2020_11_06_000006_create_item_groups_table.php 2021_02_08_000007_create_item_groups_table.php;</v>
+        <v>ren 2021_03_25_000007_create_item_groups_table.php 2021_03_25_000007_create_item_groups_table.php;</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -794,7 +794,7 @@
       </c>
       <c r="C9" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>2021_02_08_</v>
+        <v>2021_03_25_</v>
       </c>
       <c r="D9" s="1" t="str">
         <f>REPT("0",6-LEN(MATCH(Table1[[#This Row],[Name]],Table1[Name],0)))&amp;MATCH(Table1[[#This Row],[Name]],Table1[Name],0)</f>
@@ -802,11 +802,11 @@
       </c>
       <c r="E9" s="2" t="str">
         <f>Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Seq]]&amp;Table1[[#This Row],[Name]]</f>
-        <v>2021_02_08_000008_create_menus_table.php</v>
+        <v>2021_03_25_000008_create_menus_table.php</v>
       </c>
       <c r="F9" s="2" t="str">
         <f>"ren "&amp;Table1[[#This Row],[Files]]&amp;" "&amp;Table1[[#This Row],[Replace]]&amp;";"</f>
-        <v>ren 2020_11_06_000007_create_menus_table.php 2021_02_08_000008_create_menus_table.php;</v>
+        <v>ren 2021_03_25_000008_create_menus_table.php 2021_03_25_000008_create_menus_table.php;</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -819,7 +819,7 @@
       </c>
       <c r="C10" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>2021_02_08_</v>
+        <v>2021_03_25_</v>
       </c>
       <c r="D10" s="1" t="str">
         <f>REPT("0",6-LEN(MATCH(Table1[[#This Row],[Name]],Table1[Name],0)))&amp;MATCH(Table1[[#This Row],[Name]],Table1[Name],0)</f>
@@ -827,11 +827,11 @@
       </c>
       <c r="E10" s="2" t="str">
         <f>Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Seq]]&amp;Table1[[#This Row],[Name]]</f>
-        <v>2021_02_08_000009_create_price_lists_table.php</v>
+        <v>2021_03_25_000009_create_price_lists_table.php</v>
       </c>
       <c r="F10" s="2" t="str">
         <f>"ren "&amp;Table1[[#This Row],[Files]]&amp;" "&amp;Table1[[#This Row],[Replace]]&amp;";"</f>
-        <v>ren 2020_11_06_000008_create_price_lists_table.php 2021_02_08_000009_create_price_lists_table.php;</v>
+        <v>ren 2021_03_25_000009_create_price_lists_table.php 2021_03_25_000009_create_price_lists_table.php;</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -844,7 +844,7 @@
       </c>
       <c r="C11" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>2021_02_08_</v>
+        <v>2021_03_25_</v>
       </c>
       <c r="D11" s="1" t="str">
         <f>REPT("0",6-LEN(MATCH(Table1[[#This Row],[Name]],Table1[Name],0)))&amp;MATCH(Table1[[#This Row],[Name]],Table1[Name],0)</f>
@@ -852,11 +852,11 @@
       </c>
       <c r="E11" s="2" t="str">
         <f>Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Seq]]&amp;Table1[[#This Row],[Name]]</f>
-        <v>2021_02_08_000010_create_prices_table.php</v>
+        <v>2021_03_25_000010_create_prices_table.php</v>
       </c>
       <c r="F11" s="2" t="str">
         <f>"ren "&amp;Table1[[#This Row],[Files]]&amp;" "&amp;Table1[[#This Row],[Replace]]&amp;";"</f>
-        <v>ren 2020_11_06_000009_create_prices_table.php 2021_02_08_000010_create_prices_table.php;</v>
+        <v>ren 2021_03_25_000010_create_prices_table.php 2021_03_25_000010_create_prices_table.php;</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -869,7 +869,7 @@
       </c>
       <c r="C12" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>2021_02_08_</v>
+        <v>2021_03_25_</v>
       </c>
       <c r="D12" s="4" t="str">
         <f>REPT("0",6-LEN(MATCH(Table1[[#This Row],[Name]],Table1[Name],0)))&amp;MATCH(Table1[[#This Row],[Name]],Table1[Name],0)</f>
@@ -877,11 +877,11 @@
       </c>
       <c r="E12" s="4" t="str">
         <f>Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Seq]]&amp;Table1[[#This Row],[Name]]</f>
-        <v>2021_02_08_000011_create_taxes_table.php</v>
+        <v>2021_03_25_000011_create_taxes_table.php</v>
       </c>
       <c r="F12" s="4" t="str">
         <f>"ren "&amp;Table1[[#This Row],[Files]]&amp;" "&amp;Table1[[#This Row],[Replace]]&amp;";"</f>
-        <v>ren 2020_11_06_000010_create_taxes_table.php 2021_02_08_000011_create_taxes_table.php;</v>
+        <v>ren 2021_03_25_000011_create_taxes_table.php 2021_03_25_000011_create_taxes_table.php;</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -894,7 +894,7 @@
       </c>
       <c r="C13" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>2021_02_08_</v>
+        <v>2021_03_25_</v>
       </c>
       <c r="D13" s="1" t="str">
         <f>REPT("0",6-LEN(MATCH(Table1[[#This Row],[Name]],Table1[Name],0)))&amp;MATCH(Table1[[#This Row],[Name]],Table1[Name],0)</f>
@@ -902,11 +902,11 @@
       </c>
       <c r="E13" s="2" t="str">
         <f>Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Seq]]&amp;Table1[[#This Row],[Name]]</f>
-        <v>2021_02_08_000012_create_kitchens_table.php</v>
+        <v>2021_03_25_000012_create_kitchens_table.php</v>
       </c>
       <c r="F13" s="2" t="str">
         <f>"ren "&amp;Table1[[#This Row],[Files]]&amp;" "&amp;Table1[[#This Row],[Replace]]&amp;";"</f>
-        <v>ren 2020_11_06_000011_create_kitchens_table.php 2021_02_08_000012_create_kitchens_table.php;</v>
+        <v>ren 2021_03_25_000012_create_kitchens_table.php 2021_03_25_000012_create_kitchens_table.php;</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -919,7 +919,7 @@
       </c>
       <c r="C14" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>2021_02_08_</v>
+        <v>2021_03_25_</v>
       </c>
       <c r="D14" s="1" t="str">
         <f>REPT("0",6-LEN(MATCH(Table1[[#This Row],[Name]],Table1[Name],0)))&amp;MATCH(Table1[[#This Row],[Name]],Table1[Name],0)</f>
@@ -927,11 +927,11 @@
       </c>
       <c r="E14" s="2" t="str">
         <f>Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Seq]]&amp;Table1[[#This Row],[Name]]</f>
-        <v>2021_02_08_000013_create_kitchen_items_table.php</v>
+        <v>2021_03_25_000013_create_kitchen_items_table.php</v>
       </c>
       <c r="F14" s="2" t="str">
         <f>"ren "&amp;Table1[[#This Row],[Files]]&amp;" "&amp;Table1[[#This Row],[Replace]]&amp;";"</f>
-        <v>ren 2020_11_06_000012_create_kitchen_items_table.php 2021_02_08_000013_create_kitchen_items_table.php;</v>
+        <v>ren 2021_03_25_000013_create_kitchen_items_table.php 2021_03_25_000013_create_kitchen_items_table.php;</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -944,7 +944,7 @@
       </c>
       <c r="C15" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>2021_02_08_</v>
+        <v>2021_03_25_</v>
       </c>
       <c r="D15" s="1" t="str">
         <f>REPT("0",6-LEN(MATCH(Table1[[#This Row],[Name]],Table1[Name],0)))&amp;MATCH(Table1[[#This Row],[Name]],Table1[Name],0)</f>
@@ -952,11 +952,11 @@
       </c>
       <c r="E15" s="2" t="str">
         <f>Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Seq]]&amp;Table1[[#This Row],[Name]]</f>
-        <v>2021_02_08_000014_create_kitchen_statuses_table.php</v>
+        <v>2021_03_25_000014_create_kitchen_statuses_table.php</v>
       </c>
       <c r="F15" s="2" t="str">
         <f>"ren "&amp;Table1[[#This Row],[Files]]&amp;" "&amp;Table1[[#This Row],[Replace]]&amp;";"</f>
-        <v>ren 2020_11_06_000013_create_kitchen_statuses_table.php 2021_02_08_000014_create_kitchen_statuses_table.php;</v>
+        <v>ren 2021_03_25_000014_create_kitchen_statuses_table.php 2021_03_25_000014_create_kitchen_statuses_table.php;</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -969,7 +969,7 @@
       </c>
       <c r="C16" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>2021_02_08_</v>
+        <v>2021_03_25_</v>
       </c>
       <c r="D16" s="1" t="str">
         <f>REPT("0",6-LEN(MATCH(Table1[[#This Row],[Name]],Table1[Name],0)))&amp;MATCH(Table1[[#This Row],[Name]],Table1[Name],0)</f>
@@ -977,11 +977,11 @@
       </c>
       <c r="E16" s="2" t="str">
         <f>Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Seq]]&amp;Table1[[#This Row],[Name]]</f>
-        <v>2021_02_08_000015_create_customers_table.php</v>
+        <v>2021_03_25_000015_create_customers_table.php</v>
       </c>
       <c r="F16" s="2" t="str">
         <f>"ren "&amp;Table1[[#This Row],[Files]]&amp;" "&amp;Table1[[#This Row],[Replace]]&amp;";"</f>
-        <v>ren 2020_11_06_000014_create_customers_table.php 2021_02_08_000015_create_customers_table.php;</v>
+        <v>ren 2021_03_25_000015_create_customers_table.php 2021_03_25_000015_create_customers_table.php;</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -994,7 +994,7 @@
       </c>
       <c r="C17" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>2021_02_08_</v>
+        <v>2021_03_25_</v>
       </c>
       <c r="D17" s="1" t="str">
         <f>REPT("0",6-LEN(MATCH(Table1[[#This Row],[Name]],Table1[Name],0)))&amp;MATCH(Table1[[#This Row],[Name]],Table1[Name],0)</f>
@@ -1002,11 +1002,11 @@
       </c>
       <c r="E17" s="2" t="str">
         <f>Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Seq]]&amp;Table1[[#This Row],[Name]]</f>
-        <v>2021_02_08_000016_create_seatings_table.php</v>
+        <v>2021_03_25_000016_create_seatings_table.php</v>
       </c>
       <c r="F17" s="2" t="str">
         <f>"ren "&amp;Table1[[#This Row],[Files]]&amp;" "&amp;Table1[[#This Row],[Replace]]&amp;";"</f>
-        <v>ren 2020_11_06_000015_create_seatings_table.php 2021_02_08_000016_create_seatings_table.php;</v>
+        <v>ren 2021_03_25_000016_create_seatings_table.php 2021_03_25_000016_create_seatings_table.php;</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -1019,7 +1019,7 @@
       </c>
       <c r="C18" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>2021_02_08_</v>
+        <v>2021_03_25_</v>
       </c>
       <c r="D18" s="1" t="str">
         <f>REPT("0",6-LEN(MATCH(Table1[[#This Row],[Name]],Table1[Name],0)))&amp;MATCH(Table1[[#This Row],[Name]],Table1[Name],0)</f>
@@ -1027,11 +1027,11 @@
       </c>
       <c r="E18" s="2" t="str">
         <f>Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Seq]]&amp;Table1[[#This Row],[Name]]</f>
-        <v>2021_02_08_000017_create_tokens_table.php</v>
+        <v>2021_03_25_000017_create_tokens_table.php</v>
       </c>
       <c r="F18" s="2" t="str">
         <f>"ren "&amp;Table1[[#This Row],[Files]]&amp;" "&amp;Table1[[#This Row],[Replace]]&amp;";"</f>
-        <v>ren 2020_11_06_000016_create_tokens_table.php 2021_02_08_000017_create_tokens_table.php;</v>
+        <v>ren 2021_03_25_000017_create_tokens_table.php 2021_03_25_000017_create_tokens_table.php;</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -1044,7 +1044,7 @@
       </c>
       <c r="C19" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>2021_02_08_</v>
+        <v>2021_03_25_</v>
       </c>
       <c r="D19" s="4" t="str">
         <f>REPT("0",6-LEN(MATCH(Table1[[#This Row],[Name]],Table1[Name],0)))&amp;MATCH(Table1[[#This Row],[Name]],Table1[Name],0)</f>
@@ -1052,11 +1052,11 @@
       </c>
       <c r="E19" s="4" t="str">
         <f>Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Seq]]&amp;Table1[[#This Row],[Name]]</f>
-        <v>2021_02_08_000018_create_token_items_table.php</v>
+        <v>2021_03_25_000018_create_token_items_table.php</v>
       </c>
       <c r="F19" s="4" t="str">
         <f>"ren "&amp;Table1[[#This Row],[Files]]&amp;" "&amp;Table1[[#This Row],[Replace]]&amp;";"</f>
-        <v>ren 2020_11_06_000017_create_token_items_table.php 2021_02_08_000018_create_token_items_table.php;</v>
+        <v>ren 2021_03_25_000018_create_token_items_table.php 2021_03_25_000018_create_token_items_table.php;</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -1069,7 +1069,7 @@
       </c>
       <c r="C20" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>2021_02_08_</v>
+        <v>2021_03_25_</v>
       </c>
       <c r="D20" s="4" t="str">
         <f>REPT("0",6-LEN(MATCH(Table1[[#This Row],[Name]],Table1[Name],0)))&amp;MATCH(Table1[[#This Row],[Name]],Table1[Name],0)</f>
@@ -1077,11 +1077,11 @@
       </c>
       <c r="E20" s="4" t="str">
         <f>Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Seq]]&amp;Table1[[#This Row],[Name]]</f>
-        <v>2021_02_08_000019_create_bills_table.php</v>
+        <v>2021_03_25_000019_create_bills_table.php</v>
       </c>
       <c r="F20" s="4" t="str">
         <f>"ren "&amp;Table1[[#This Row],[Files]]&amp;" "&amp;Table1[[#This Row],[Replace]]&amp;";"</f>
-        <v>ren 2020_11_06_000018_create_bills_table.php 2021_02_08_000019_create_bills_table.php;</v>
+        <v>ren 2021_03_25_000019_create_bills_table.php 2021_03_25_000019_create_bills_table.php;</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -1094,7 +1094,7 @@
       </c>
       <c r="C21" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>2021_02_08_</v>
+        <v>2021_03_25_</v>
       </c>
       <c r="D21" s="4" t="str">
         <f>REPT("0",6-LEN(MATCH(Table1[[#This Row],[Name]],Table1[Name],0)))&amp;MATCH(Table1[[#This Row],[Name]],Table1[Name],0)</f>
@@ -1102,24 +1102,24 @@
       </c>
       <c r="E21" s="4" t="str">
         <f>Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Seq]]&amp;Table1[[#This Row],[Name]]</f>
-        <v>2021_02_08_000020_create_payments_table.php</v>
+        <v>2021_03_25_000020_create_payments_table.php</v>
       </c>
       <c r="F21" s="4" t="str">
         <f>"ren "&amp;Table1[[#This Row],[Files]]&amp;" "&amp;Table1[[#This Row],[Replace]]&amp;";"</f>
-        <v>ren 2020_11_06_000019_create_payments_table.php 2021_02_08_000020_create_payments_table.php;</v>
+        <v>ren 2021_03_25_000020_create_payments_table.php 2021_03_25_000020_create_payments_table.php;</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B22" s="4" t="str">
         <f>MID(Table1[[#This Row],[Files]],18,LEN(Table1[[#This Row],[Files]]))</f>
-        <v>_create_remote_items_table.php</v>
+        <v>_create_remote_table.php</v>
       </c>
       <c r="C22" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>2021_02_08_</v>
+        <v>2021_03_25_</v>
       </c>
       <c r="D22" s="4" t="str">
         <f>REPT("0",6-LEN(MATCH(Table1[[#This Row],[Name]],Table1[Name],0)))&amp;MATCH(Table1[[#This Row],[Name]],Table1[Name],0)</f>
@@ -1127,11 +1127,11 @@
       </c>
       <c r="E22" s="4" t="str">
         <f>Table1[[#This Row],[Date]]&amp;Table1[[#This Row],[Seq]]&amp;Table1[[#This Row],[Name]]</f>
-        <v>2021_02_08_000021_create_remote_items_table.php</v>
+        <v>2021_03_25_000021_create_remote_table.php</v>
       </c>
       <c r="F22" s="4" t="str">
         <f>"ren "&amp;Table1[[#This Row],[Files]]&amp;" "&amp;Table1[[#This Row],[Replace]]&amp;";"</f>
-        <v>ren 2020_11_06_000021_create_remote_items_table.php 2021_02_08_000021_create_remote_items_table.php;</v>
+        <v>ren 2021_03_25_000021_create_remote_table.php 2021_03_25_000021_create_remote_table.php;</v>
       </c>
     </row>
   </sheetData>

</xml_diff>